<commit_message>
build the sv events from vcf files
</commit_message>
<xml_diff>
--- a/GeneTarget/server/metadata.xlsx
+++ b/GeneTarget/server/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\hackathon\NeuroSV\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mostafa\GeneTarget\GeneTarget\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01EF6AD-F5C6-4FE3-B6CE-531CAE051CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0BE58-DE5C-4720-A66C-B7A7D3391F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BDF8D68-BE9A-9E4A-A515-1221F880875C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BDF8D68-BE9A-9E4A-A515-1221F880875C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,208 +134,208 @@
     <t>ERBB4</t>
   </si>
   <si>
-    <t>LP6005878-DNA_A01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_A09.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_B09.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_C09.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_D08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_E08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_F08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_G08.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H01.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H02.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H03.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H04.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H05.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H06.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H07.SV.vcf.gz</t>
-  </si>
-  <si>
-    <t>LP6005878-DNA_H08.SV.vcf.gz</t>
-  </si>
-  <si>
     <t>patient_ID</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_A09</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_B09</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_C09</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_D08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_E08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_F08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_G08</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H01</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H02</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H03</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H04</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H05</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H06</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H07</t>
+  </si>
+  <si>
+    <t>LP6005878-DNA_H08</t>
   </si>
 </sst>
 </file>
@@ -697,15 +697,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005DD06C-617E-E24C-8013-5760C81D8236}">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E34" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -777,9 +780,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -851,9 +854,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -925,9 +928,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -999,9 +1002,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1073,9 +1076,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1147,9 +1150,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1221,9 +1224,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1295,9 +1298,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1369,9 +1372,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1443,9 +1446,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1517,9 +1520,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1591,9 +1594,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1665,9 +1668,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1739,9 +1742,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1813,9 +1816,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1887,9 +1890,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1961,9 +1964,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2035,9 +2038,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2109,9 +2112,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2183,9 +2186,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2257,9 +2260,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2331,9 +2334,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2405,9 +2408,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2479,9 +2482,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2553,9 +2556,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2627,9 +2630,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -2701,9 +2704,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2775,9 +2778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -2849,9 +2852,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2923,9 +2926,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -2997,9 +3000,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3071,9 +3074,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -3145,9 +3148,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3219,9 +3222,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3293,9 +3296,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3367,9 +3370,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3441,9 +3444,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3515,9 +3518,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3589,9 +3592,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -3663,9 +3666,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3737,9 +3740,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -3811,9 +3814,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -3885,9 +3888,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3959,9 +3962,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4033,9 +4036,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4107,9 +4110,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4181,9 +4184,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4255,9 +4258,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4329,9 +4332,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4403,9 +4406,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4477,9 +4480,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4551,9 +4554,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4625,9 +4628,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4699,9 +4702,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4773,9 +4776,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -4847,9 +4850,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -4921,9 +4924,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4995,9 +4998,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -5069,9 +5072,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -5143,9 +5146,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -5217,9 +5220,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -5291,9 +5294,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -5365,9 +5368,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -5439,9 +5442,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -5513,9 +5516,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -5587,9 +5590,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -5661,9 +5664,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <v>1</v>

</xml_diff>